<commit_message>
Added Display class Updated images
</commit_message>
<xml_diff>
--- a/src/WebMarket/WebMarket/App_Data/Charger.xlsx
+++ b/src/WebMarket/WebMarket/App_Data/Charger.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -31,12 +31,6 @@
     <t>Producer</t>
   </si>
   <si>
-    <t>IsTopBuyed</t>
-  </si>
-  <si>
-    <t>IsNew</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -95,6 +89,9 @@
   </si>
   <si>
     <t>Availability</t>
+  </si>
+  <si>
+    <t>DisplayClass</t>
   </si>
 </sst>
 </file>
@@ -435,15 +432,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,7 +451,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -463,51 +460,48 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>15</v>
-      </c>
-      <c r="T1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
       </c>
       <c r="B2">
         <v>15.6</v>
@@ -516,53 +510,53 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2">
+        <v>24</v>
+      </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="S2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>18</v>
-      </c>
-      <c r="J2">
-        <v>24</v>
-      </c>
-      <c r="K2">
-        <v>5</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="T2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="I3">
+        <v>24</v>
       </c>
       <c r="J3">
-        <v>24</v>
-      </c>
-      <c r="K3">
         <v>5</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="R3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>19</v>
-      </c>
-      <c r="T3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
       </c>
       <c r="B4">
         <v>18</v>
@@ -571,27 +565,27 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4">
+        <v>24</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4">
-        <v>24</v>
-      </c>
-      <c r="K4">
-        <v>5</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="T4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>23</v>
       </c>
       <c r="B5">
         <v>27</v>
@@ -600,21 +594,21 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="I5">
+        <v>24</v>
       </c>
       <c r="J5">
-        <v>24</v>
-      </c>
-      <c r="K5">
         <v>5</v>
       </c>
-      <c r="S5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="T5">
+      <c r="R5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S5">
         <v>12</v>
       </c>
     </row>

</xml_diff>